<commit_message>
Added calib. curv fit and jig shape sensing
Signed-off-by: Dimitri Lezcano <dlezcan1@jhu.edu>
</commit_message>
<xml_diff>
--- a/FBG_Needle_Calibration_Data/needle_3CH_4AA/Validation_Jig_Calibration_08-19-20/Data Matrices_proc.xlsx
+++ b/FBG_Needle_Calibration_Data/needle_3CH_4AA/Validation_Jig_Calibration_08-19-20/Data Matrices_proc.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="956" uniqueCount="23">
   <si>
     <t>Var1</t>
   </si>
@@ -106,7 +106,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="25">
+  <borders count="97">
     <border>
       <left/>
       <right/>
@@ -138,11 +138,83 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="97">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -168,6 +240,78 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="33" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="34" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="35" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="36" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="37" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="38" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="39" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="40" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="41" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="42" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="43" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="44" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="45" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="46" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="47" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="48" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="49" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="50" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="51" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="52" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="53" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="54" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="55" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="56" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="57" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="58" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="59" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="60" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="61" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="62" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="63" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="64" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="65" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="66" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="67" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="68" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="69" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="70" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="71" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="72" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="73" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="74" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="75" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="76" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="77" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="78" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="79" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="80" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="81" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="82" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="83" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="84" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="85" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="86" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="87" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="88" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="89" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="90" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="91" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="92" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="93" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="94" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="95" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="96" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -193,39 +337,39 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="89" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="89" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="89" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="D1" s="89" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="17" t="s">
+      <c r="E1" s="89" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="17" t="s">
+      <c r="F1" s="89" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="17" t="s">
+      <c r="G1" s="89" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="17" t="s">
+      <c r="H1" s="89" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="17" t="s">
+      <c r="I1" s="89" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="17" t="s">
+      <c r="J1" s="89" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="89" t="s">
         <v>11</v>
       </c>
       <c r="B2">
@@ -257,7 +401,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="89" t="s">
         <v>12</v>
       </c>
       <c r="B3">
@@ -289,7 +433,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="17" t="s">
+      <c r="A4" s="89" t="s">
         <v>13</v>
       </c>
       <c r="B4">
@@ -321,7 +465,7 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="17" t="s">
+      <c r="A5" s="89" t="s">
         <v>14</v>
       </c>
       <c r="B5">
@@ -353,7 +497,7 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="17" t="s">
+      <c r="A6" s="89" t="s">
         <v>15</v>
       </c>
       <c r="B6">
@@ -385,7 +529,7 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="17" t="s">
+      <c r="A7" s="89" t="s">
         <v>16</v>
       </c>
       <c r="B7">
@@ -417,7 +561,7 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="17" t="s">
+      <c r="A8" s="89" t="s">
         <v>17</v>
       </c>
       <c r="B8">
@@ -449,7 +593,7 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="17" t="s">
+      <c r="A9" s="89" t="s">
         <v>18</v>
       </c>
       <c r="B9">
@@ -481,7 +625,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="17" t="s">
+      <c r="A10" s="89" t="s">
         <v>19</v>
       </c>
       <c r="B10">
@@ -513,7 +657,7 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="17" t="s">
+      <c r="A11" s="89" t="s">
         <v>20</v>
       </c>
       <c r="B11">
@@ -545,7 +689,7 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="17" t="s">
+      <c r="A12" s="89" t="s">
         <v>21</v>
       </c>
       <c r="B12">
@@ -577,7 +721,7 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="17" t="s">
+      <c r="A13" s="89" t="s">
         <v>22</v>
       </c>
       <c r="B13">
@@ -630,39 +774,39 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="91" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="91" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="91" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="D1" s="91" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="19" t="s">
+      <c r="E1" s="91" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="19" t="s">
+      <c r="F1" s="91" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="19" t="s">
+      <c r="G1" s="91" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="19" t="s">
+      <c r="H1" s="91" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="19" t="s">
+      <c r="I1" s="91" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="19" t="s">
+      <c r="J1" s="91" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="91" t="s">
         <v>11</v>
       </c>
       <c r="B2">
@@ -694,7 +838,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="91" t="s">
         <v>12</v>
       </c>
       <c r="B3">
@@ -726,7 +870,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="19" t="s">
+      <c r="A4" s="91" t="s">
         <v>13</v>
       </c>
       <c r="B4">
@@ -758,7 +902,7 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="19" t="s">
+      <c r="A5" s="91" t="s">
         <v>14</v>
       </c>
       <c r="B5">
@@ -790,7 +934,7 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="19" t="s">
+      <c r="A6" s="91" t="s">
         <v>15</v>
       </c>
       <c r="B6">
@@ -822,7 +966,7 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="19" t="s">
+      <c r="A7" s="91" t="s">
         <v>16</v>
       </c>
       <c r="B7">
@@ -854,7 +998,7 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="19" t="s">
+      <c r="A8" s="91" t="s">
         <v>17</v>
       </c>
       <c r="B8">
@@ -886,7 +1030,7 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="19" t="s">
+      <c r="A9" s="91" t="s">
         <v>18</v>
       </c>
       <c r="B9">
@@ -918,7 +1062,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="19" t="s">
+      <c r="A10" s="91" t="s">
         <v>19</v>
       </c>
       <c r="B10">
@@ -950,7 +1094,7 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="19" t="s">
+      <c r="A11" s="91" t="s">
         <v>20</v>
       </c>
       <c r="B11">
@@ -982,7 +1126,7 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="19" t="s">
+      <c r="A12" s="91" t="s">
         <v>21</v>
       </c>
       <c r="B12">
@@ -1014,7 +1158,7 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="19" t="s">
+      <c r="A13" s="91" t="s">
         <v>22</v>
       </c>
       <c r="B13">
@@ -1067,39 +1211,39 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="93" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="93" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="93" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="D1" s="93" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="21" t="s">
+      <c r="E1" s="93" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="21" t="s">
+      <c r="F1" s="93" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="21" t="s">
+      <c r="G1" s="93" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="21" t="s">
+      <c r="H1" s="93" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="21" t="s">
+      <c r="I1" s="93" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="21" t="s">
+      <c r="J1" s="93" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="93" t="s">
         <v>11</v>
       </c>
       <c r="B2">
@@ -1131,7 +1275,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="93" t="s">
         <v>12</v>
       </c>
       <c r="B3">
@@ -1163,7 +1307,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="21" t="s">
+      <c r="A4" s="93" t="s">
         <v>13</v>
       </c>
       <c r="B4">
@@ -1195,7 +1339,7 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="21" t="s">
+      <c r="A5" s="93" t="s">
         <v>14</v>
       </c>
       <c r="B5">
@@ -1227,7 +1371,7 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="21" t="s">
+      <c r="A6" s="93" t="s">
         <v>15</v>
       </c>
       <c r="B6">
@@ -1259,7 +1403,7 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="21" t="s">
+      <c r="A7" s="93" t="s">
         <v>16</v>
       </c>
       <c r="B7">
@@ -1291,7 +1435,7 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="21" t="s">
+      <c r="A8" s="93" t="s">
         <v>17</v>
       </c>
       <c r="B8">
@@ -1323,7 +1467,7 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="21" t="s">
+      <c r="A9" s="93" t="s">
         <v>18</v>
       </c>
       <c r="B9">
@@ -1355,7 +1499,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="21" t="s">
+      <c r="A10" s="93" t="s">
         <v>19</v>
       </c>
       <c r="B10">
@@ -1387,7 +1531,7 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="21" t="s">
+      <c r="A11" s="93" t="s">
         <v>20</v>
       </c>
       <c r="B11">
@@ -1419,7 +1563,7 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="21" t="s">
+      <c r="A12" s="93" t="s">
         <v>21</v>
       </c>
       <c r="B12">
@@ -1451,7 +1595,7 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="21" t="s">
+      <c r="A13" s="93" t="s">
         <v>22</v>
       </c>
       <c r="B13">
@@ -1504,39 +1648,39 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="95" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="95" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="23" t="s">
+      <c r="C1" s="95" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="23" t="s">
+      <c r="D1" s="95" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="23" t="s">
+      <c r="E1" s="95" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="23" t="s">
+      <c r="F1" s="95" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="23" t="s">
+      <c r="G1" s="95" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="23" t="s">
+      <c r="H1" s="95" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="23" t="s">
+      <c r="I1" s="95" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="23" t="s">
+      <c r="J1" s="95" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="95" t="s">
         <v>11</v>
       </c>
       <c r="B2">
@@ -1568,7 +1712,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="23" t="s">
+      <c r="A3" s="95" t="s">
         <v>12</v>
       </c>
       <c r="B3">
@@ -1600,7 +1744,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="23" t="s">
+      <c r="A4" s="95" t="s">
         <v>13</v>
       </c>
       <c r="B4">
@@ -1632,7 +1776,7 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="23" t="s">
+      <c r="A5" s="95" t="s">
         <v>14</v>
       </c>
       <c r="B5">
@@ -1664,7 +1808,7 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="23" t="s">
+      <c r="A6" s="95" t="s">
         <v>15</v>
       </c>
       <c r="B6">
@@ -1696,7 +1840,7 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="23" t="s">
+      <c r="A7" s="95" t="s">
         <v>16</v>
       </c>
       <c r="B7">
@@ -1728,7 +1872,7 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="23" t="s">
+      <c r="A8" s="95" t="s">
         <v>17</v>
       </c>
       <c r="B8">
@@ -1760,7 +1904,7 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="23" t="s">
+      <c r="A9" s="95" t="s">
         <v>18</v>
       </c>
       <c r="B9">
@@ -1792,7 +1936,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="23" t="s">
+      <c r="A10" s="95" t="s">
         <v>19</v>
       </c>
       <c r="B10">
@@ -1824,7 +1968,7 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="23" t="s">
+      <c r="A11" s="95" t="s">
         <v>20</v>
       </c>
       <c r="B11">
@@ -1856,7 +2000,7 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="23" t="s">
+      <c r="A12" s="95" t="s">
         <v>21</v>
       </c>
       <c r="B12">
@@ -1888,7 +2032,7 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="23" t="s">
+      <c r="A13" s="95" t="s">
         <v>22</v>
       </c>
       <c r="B13">

</xml_diff>

<commit_message>
Added in-plane error for 2-D shape sensing
Signed-off-by: Dimitri Lezcano <dlezcan1@jhu.edu>
</commit_message>
<xml_diff>
--- a/FBG_Needle_Calibration_Data/needle_3CH_4AA/Validation_Jig_Calibration_08-19-20/Data Matrices_proc.xlsx
+++ b/FBG_Needle_Calibration_Data/needle_3CH_4AA/Validation_Jig_Calibration_08-19-20/Data Matrices_proc.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="956" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1044" uniqueCount="23">
   <si>
     <t>Var1</t>
   </si>
@@ -106,7 +106,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="97">
+  <borders count="105">
     <border>
       <left/>
       <right/>
@@ -210,11 +210,19 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="97">
+  <cellXfs count="105">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -312,6 +320,14 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="94" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="95" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="96" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="97" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="98" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="99" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="100" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="101" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="102" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="103" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="104" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -337,39 +353,39 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="89" t="s">
+      <c r="A1" s="97" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="89" t="s">
+      <c r="B1" s="97" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="89" t="s">
+      <c r="C1" s="97" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="89" t="s">
+      <c r="D1" s="97" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="89" t="s">
+      <c r="E1" s="97" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="89" t="s">
+      <c r="F1" s="97" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="89" t="s">
+      <c r="G1" s="97" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="89" t="s">
+      <c r="H1" s="97" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="89" t="s">
+      <c r="I1" s="97" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="89" t="s">
+      <c r="J1" s="97" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="89" t="s">
+      <c r="A2" s="97" t="s">
         <v>11</v>
       </c>
       <c r="B2">
@@ -401,7 +417,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="89" t="s">
+      <c r="A3" s="97" t="s">
         <v>12</v>
       </c>
       <c r="B3">
@@ -433,7 +449,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="89" t="s">
+      <c r="A4" s="97" t="s">
         <v>13</v>
       </c>
       <c r="B4">
@@ -465,7 +481,7 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="89" t="s">
+      <c r="A5" s="97" t="s">
         <v>14</v>
       </c>
       <c r="B5">
@@ -497,7 +513,7 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="89" t="s">
+      <c r="A6" s="97" t="s">
         <v>15</v>
       </c>
       <c r="B6">
@@ -529,7 +545,7 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="89" t="s">
+      <c r="A7" s="97" t="s">
         <v>16</v>
       </c>
       <c r="B7">
@@ -561,7 +577,7 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="89" t="s">
+      <c r="A8" s="97" t="s">
         <v>17</v>
       </c>
       <c r="B8">
@@ -593,7 +609,7 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="89" t="s">
+      <c r="A9" s="97" t="s">
         <v>18</v>
       </c>
       <c r="B9">
@@ -625,7 +641,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="89" t="s">
+      <c r="A10" s="97" t="s">
         <v>19</v>
       </c>
       <c r="B10">
@@ -657,7 +673,7 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="89" t="s">
+      <c r="A11" s="97" t="s">
         <v>20</v>
       </c>
       <c r="B11">
@@ -689,7 +705,7 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="89" t="s">
+      <c r="A12" s="97" t="s">
         <v>21</v>
       </c>
       <c r="B12">
@@ -721,7 +737,7 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="89" t="s">
+      <c r="A13" s="97" t="s">
         <v>22</v>
       </c>
       <c r="B13">
@@ -774,39 +790,39 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="91" t="s">
+      <c r="A1" s="99" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="91" t="s">
+      <c r="B1" s="99" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="91" t="s">
+      <c r="C1" s="99" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="91" t="s">
+      <c r="D1" s="99" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="91" t="s">
+      <c r="E1" s="99" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="91" t="s">
+      <c r="F1" s="99" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="91" t="s">
+      <c r="G1" s="99" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="91" t="s">
+      <c r="H1" s="99" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="91" t="s">
+      <c r="I1" s="99" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="91" t="s">
+      <c r="J1" s="99" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="91" t="s">
+      <c r="A2" s="99" t="s">
         <v>11</v>
       </c>
       <c r="B2">
@@ -838,7 +854,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="91" t="s">
+      <c r="A3" s="99" t="s">
         <v>12</v>
       </c>
       <c r="B3">
@@ -870,7 +886,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="91" t="s">
+      <c r="A4" s="99" t="s">
         <v>13</v>
       </c>
       <c r="B4">
@@ -902,7 +918,7 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="91" t="s">
+      <c r="A5" s="99" t="s">
         <v>14</v>
       </c>
       <c r="B5">
@@ -934,7 +950,7 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="91" t="s">
+      <c r="A6" s="99" t="s">
         <v>15</v>
       </c>
       <c r="B6">
@@ -966,7 +982,7 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="91" t="s">
+      <c r="A7" s="99" t="s">
         <v>16</v>
       </c>
       <c r="B7">
@@ -998,7 +1014,7 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="91" t="s">
+      <c r="A8" s="99" t="s">
         <v>17</v>
       </c>
       <c r="B8">
@@ -1030,7 +1046,7 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="91" t="s">
+      <c r="A9" s="99" t="s">
         <v>18</v>
       </c>
       <c r="B9">
@@ -1062,7 +1078,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="91" t="s">
+      <c r="A10" s="99" t="s">
         <v>19</v>
       </c>
       <c r="B10">
@@ -1094,7 +1110,7 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="91" t="s">
+      <c r="A11" s="99" t="s">
         <v>20</v>
       </c>
       <c r="B11">
@@ -1126,7 +1142,7 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="91" t="s">
+      <c r="A12" s="99" t="s">
         <v>21</v>
       </c>
       <c r="B12">
@@ -1158,7 +1174,7 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="91" t="s">
+      <c r="A13" s="99" t="s">
         <v>22</v>
       </c>
       <c r="B13">
@@ -1211,39 +1227,39 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="93" t="s">
+      <c r="A1" s="101" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="93" t="s">
+      <c r="B1" s="101" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="93" t="s">
+      <c r="C1" s="101" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="93" t="s">
+      <c r="D1" s="101" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="93" t="s">
+      <c r="E1" s="101" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="93" t="s">
+      <c r="F1" s="101" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="93" t="s">
+      <c r="G1" s="101" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="93" t="s">
+      <c r="H1" s="101" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="93" t="s">
+      <c r="I1" s="101" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="93" t="s">
+      <c r="J1" s="101" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="93" t="s">
+      <c r="A2" s="101" t="s">
         <v>11</v>
       </c>
       <c r="B2">
@@ -1275,7 +1291,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="93" t="s">
+      <c r="A3" s="101" t="s">
         <v>12</v>
       </c>
       <c r="B3">
@@ -1307,7 +1323,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="93" t="s">
+      <c r="A4" s="101" t="s">
         <v>13</v>
       </c>
       <c r="B4">
@@ -1339,7 +1355,7 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="93" t="s">
+      <c r="A5" s="101" t="s">
         <v>14</v>
       </c>
       <c r="B5">
@@ -1371,7 +1387,7 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="93" t="s">
+      <c r="A6" s="101" t="s">
         <v>15</v>
       </c>
       <c r="B6">
@@ -1403,7 +1419,7 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="93" t="s">
+      <c r="A7" s="101" t="s">
         <v>16</v>
       </c>
       <c r="B7">
@@ -1435,7 +1451,7 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="93" t="s">
+      <c r="A8" s="101" t="s">
         <v>17</v>
       </c>
       <c r="B8">
@@ -1467,7 +1483,7 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="93" t="s">
+      <c r="A9" s="101" t="s">
         <v>18</v>
       </c>
       <c r="B9">
@@ -1499,7 +1515,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="93" t="s">
+      <c r="A10" s="101" t="s">
         <v>19</v>
       </c>
       <c r="B10">
@@ -1531,7 +1547,7 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="93" t="s">
+      <c r="A11" s="101" t="s">
         <v>20</v>
       </c>
       <c r="B11">
@@ -1563,7 +1579,7 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="93" t="s">
+      <c r="A12" s="101" t="s">
         <v>21</v>
       </c>
       <c r="B12">
@@ -1595,7 +1611,7 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="93" t="s">
+      <c r="A13" s="101" t="s">
         <v>22</v>
       </c>
       <c r="B13">
@@ -1648,39 +1664,39 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="95" t="s">
+      <c r="A1" s="103" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="95" t="s">
+      <c r="B1" s="103" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="95" t="s">
+      <c r="C1" s="103" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="95" t="s">
+      <c r="D1" s="103" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="95" t="s">
+      <c r="E1" s="103" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="95" t="s">
+      <c r="F1" s="103" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="95" t="s">
+      <c r="G1" s="103" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="95" t="s">
+      <c r="H1" s="103" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="95" t="s">
+      <c r="I1" s="103" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="95" t="s">
+      <c r="J1" s="103" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="95" t="s">
+      <c r="A2" s="103" t="s">
         <v>11</v>
       </c>
       <c r="B2">
@@ -1712,7 +1728,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="95" t="s">
+      <c r="A3" s="103" t="s">
         <v>12</v>
       </c>
       <c r="B3">
@@ -1744,7 +1760,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="95" t="s">
+      <c r="A4" s="103" t="s">
         <v>13</v>
       </c>
       <c r="B4">
@@ -1776,7 +1792,7 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="95" t="s">
+      <c r="A5" s="103" t="s">
         <v>14</v>
       </c>
       <c r="B5">
@@ -1808,7 +1824,7 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="95" t="s">
+      <c r="A6" s="103" t="s">
         <v>15</v>
       </c>
       <c r="B6">
@@ -1840,7 +1856,7 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="95" t="s">
+      <c r="A7" s="103" t="s">
         <v>16</v>
       </c>
       <c r="B7">
@@ -1872,7 +1888,7 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="95" t="s">
+      <c r="A8" s="103" t="s">
         <v>17</v>
       </c>
       <c r="B8">
@@ -1904,7 +1920,7 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="95" t="s">
+      <c r="A9" s="103" t="s">
         <v>18</v>
       </c>
       <c r="B9">
@@ -1936,7 +1952,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="95" t="s">
+      <c r="A10" s="103" t="s">
         <v>19</v>
       </c>
       <c r="B10">
@@ -1968,7 +1984,7 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="95" t="s">
+      <c r="A11" s="103" t="s">
         <v>20</v>
       </c>
       <c r="B11">
@@ -2000,7 +2016,7 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="95" t="s">
+      <c r="A12" s="103" t="s">
         <v>21</v>
       </c>
       <c r="B12">
@@ -2032,7 +2048,7 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="95" t="s">
+      <c r="A13" s="103" t="s">
         <v>22</v>
       </c>
       <c r="B13">

</xml_diff>